<commit_message>
update summary and README.md
</commit_message>
<xml_diff>
--- a/result/summary.xlsx
+++ b/result/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\내 드라이브\DnClab\papers\sc19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2450126F-FA7A-4C2D-A659-C76E592D8930}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372E44D2-9DAC-4AC9-945B-7089C8C25AEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="945" yWindow="-120" windowWidth="27975" windowHeight="16440" xr2:uid="{EB71D1F4-F278-47FB-9B1B-CD7E53CD08E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>R/T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If applied our proposed system</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Exe.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,13 +287,48 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -293,17 +340,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
+    <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3968,10 +4032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5221FBC-7FEC-4905-A474-1038BDAF9C93}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z45" sqref="Z45"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6052,6 +6116,9 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>64</v>
+      </c>
       <c r="K38">
         <f t="shared" ref="K38:M38" si="4">SUM(K2:K37)</f>
         <v>88219</v>
@@ -6069,52 +6136,97 @@
         <v>126005</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J39" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
         <v>59</v>
       </c>
-      <c r="K39">
+      <c r="K40">
         <f>K38+M38</f>
         <v>111061</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J40" t="s">
-        <v>60</v>
-      </c>
-      <c r="K40">
-        <f>K38/N38</f>
-        <v>0.70012301099162733</v>
-      </c>
+      <c r="M40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K41">
-        <f>M38/N38</f>
-        <v>0.18127852069362327</v>
+        <f>K38/N38</f>
+        <v>0.70012301099162733</v>
+      </c>
+      <c r="M41" t="s">
+        <v>59</v>
+      </c>
+      <c r="N41">
+        <f>K2+M37</f>
+        <v>5300</v>
+      </c>
+      <c r="P41" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q41" s="2">
+        <f>N41/N43</f>
+        <v>0.26188358533451922</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K42">
-        <f>(K38+M38)/N38</f>
-        <v>0.88140153168525059</v>
+        <f>M38/N38</f>
+        <v>0.18127852069362327</v>
+      </c>
+      <c r="M42" t="s">
+        <v>58</v>
+      </c>
+      <c r="N42">
+        <f>SUM(L2:L37)</f>
+        <v>14938</v>
+      </c>
+      <c r="P42" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q42">
+        <f>N42/N43</f>
+        <v>0.73811641466548072</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J43" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43" s="1">
+        <f>(K38+M38)/N38</f>
+        <v>0.88140153168525059</v>
+      </c>
+      <c r="M43" t="s">
+        <v>66</v>
+      </c>
+      <c r="N43">
+        <f>N41+N42</f>
+        <v>20238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
         <v>63</v>
       </c>
-      <c r="K43">
+      <c r="K44">
         <f>L38/N38</f>
         <v>0.11855085115670014</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M40:Q40"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>